<commit_message>
Updating jacoco csv and Codec Calculations (All Metrics)
</commit_message>
<xml_diff>
--- a/Metrics Calculations/Project 2 - Apache Commons Codec/Apache Commons Codec Calculations(All Metrics).xlsx
+++ b/Metrics Calculations/Project 2 - Apache Commons Codec/Apache Commons Codec Calculations(All Metrics).xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkhas\OneDrive\Desktop\SM Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicky\Desktop\SM\SOEN6611-Project\SoftwareMeasurement\Metrics Calculations\Project 2 - Apache Commons Codec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2881E9CB-B0EC-4123-B17C-00071D218FC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{50E3CEFD-E73F-4B77-89F5-5FCB44682E92}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Codec" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Khashyap V</author>
   </authors>
   <commentList>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{76E5B641-ECA1-4116-A43A-E070ABEA85BC}">
+    <comment ref="N8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,12 +367,6 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,6 +390,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
@@ -719,11 +718,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D8104E-90BB-4E2F-A384-70DC1C07447A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,179 +741,197 @@
   <sheetData>
     <row r="1" spans="2:27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" s="1" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="2:27" s="1" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="I3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" spans="2:27" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>1.1200000000000001</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="6">
         <v>1.1100000000000001</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="5">
         <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="5" spans="2:27" s="1" customFormat="1" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="AA5"/>
     </row>
     <row r="6" spans="2:27" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="12"/>
-      <c r="I6" s="4" t="s">
+      <c r="D6" s="7">
+        <v>96</v>
+      </c>
+      <c r="E6" s="8">
+        <v>96</v>
+      </c>
+      <c r="F6" s="10">
+        <v>96</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="8">
         <v>21827</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="8">
         <v>22362</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="8">
         <v>22362</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="8">
         <v>22359</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="10">
         <v>22359</v>
       </c>
       <c r="AA6"/>
     </row>
     <row r="7" spans="2:27" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="I7" s="4" t="s">
+      <c r="D7" s="7">
+        <v>92</v>
+      </c>
+      <c r="E7" s="8">
+        <v>91</v>
+      </c>
+      <c r="F7" s="9">
+        <v>89</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="8">
         <v>1056</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="8">
         <v>2</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="8">
         <v>5</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="9">
         <v>0</v>
       </c>
       <c r="AA7"/>
     </row>
     <row r="8" spans="2:27" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="I8" s="4" t="s">
+      <c r="D8" s="7">
+        <v>1733</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1868</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1989</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="9">
         <f>(K7+L7+M7)/N6</f>
         <v>4.7542376671586388E-2</v>
       </c>
@@ -922,147 +939,165 @@
     </row>
     <row r="9" spans="2:27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:27" s="1" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="I10" s="3" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="I10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
     </row>
     <row r="11" spans="2:27" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>1.1200000000000001</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="5">
         <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="12" spans="2:27" s="1" customFormat="1" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:27" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12"/>
-      <c r="I13" s="4" t="s">
+      <c r="D13" s="7">
+        <v>45</v>
+      </c>
+      <c r="E13" s="8">
+        <v>50</v>
+      </c>
+      <c r="F13" s="10">
+        <v>52</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="7">
         <v>26</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="8">
         <v>6</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:27" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="I14" s="4" t="s">
+      <c r="D14" s="7">
+        <v>95</v>
+      </c>
+      <c r="E14" s="8">
+        <v>92</v>
+      </c>
+      <c r="F14" s="9">
+        <v>92</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="7">
         <v>19269</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="8">
         <v>21827</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="10">
         <v>22359</v>
       </c>
     </row>
     <row r="15" spans="2:27" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="I15" s="4" t="s">
+      <c r="D15" s="7">
+        <v>90</v>
+      </c>
+      <c r="E15" s="8">
+        <v>87</v>
+      </c>
+      <c r="F15" s="9">
+        <v>87</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="7">
         <f>J13/J14</f>
         <v>1.3493175566972858E-3</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="7">
         <f>K13/K14</f>
         <v>2.748888990699592E-4</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="9">
         <f>L13/L14</f>
         <v>1.3417415805715819E-4</v>
       </c>
     </row>
     <row r="16" spans="2:27" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="7">
         <f>J15*1000</f>
         <v>1.3493175566972857</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="7">
         <f>K15*1000</f>
         <v>0.27488889906995922</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="9">
         <f>L15*1000</f>
         <v>0.13417415805715818</v>
       </c>
@@ -1132,12 +1167,12 @@
     <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B17:O17"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="I10:L10"/>
-    <mergeCell ref="B17:O17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>